<commit_message>
Version Feb 5, 2022
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/based_modeling_trial.xlsx
+++ b/data_driven/modeling/output/based_modeling_trial.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t xml:space="preserve">Param ID</t>
   </si>
@@ -143,6 +143,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -333,10 +334,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -413,32 +414,108 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>0.43</v>
+      <c r="D3" s="4" t="n">
+        <v>0.4</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>0.8</v>
+        <v>0.77</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="3" t="n">
-        <v>0.43</v>
+      <c r="G3" s="4" t="n">
+        <v>0.4</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I3" s="3" t="n">
-        <v>0.57</v>
+        <v>0.77</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>0.6</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0.004</v>
+        <v>0.001493</v>
       </c>
       <c r="K3" s="4" t="n">
         <v>0.9</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>0</v>
+        <v>0.001789</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>0.001342</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0.000575</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>0.001138</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0.000831</v>
       </c>
     </row>
   </sheetData>
@@ -467,7 +544,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -477,9 +554,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="16.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="6" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="21.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="14" style="6" width="11.52"/>
   </cols>
   <sheetData>
@@ -553,7 +630,8 @@
       <c r="A3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="b">
+      <c r="B3" s="9" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C3" s="8" t="n">
@@ -592,7 +670,8 @@
       <c r="N3" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="O3" s="9" t="b">
+      <c r="O3" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -603,7 +682,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Version Feb 09, 2022
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/based_modeling_trial.xlsx
+++ b/data_driven/modeling/output/based_modeling_trial.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t xml:space="preserve">Param ID</t>
   </si>
@@ -36,6 +36,15 @@
   </si>
   <si>
     <t xml:space="preserve">Y-randomization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time consumed (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time/N samples</t>
   </si>
   <si>
     <t xml:space="preserve">Mean validation accuracy</t>
@@ -136,14 +145,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,13 +168,25 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -216,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,6 +245,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,11 +265,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,7 +312,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -334,10 +362,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,160 +399,205 @@
         <v>4</v>
       </c>
       <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="n">
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="5" t="n">
         <v>0.77</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="4" t="n">
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="5" t="n">
         <v>0.77</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" s="6" t="n">
         <v>0.001493</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="5" t="n">
         <v>0.9</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="6" t="n">
         <v>0.001789</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>208</v>
+      </c>
+      <c r="N3" s="4" t="n">
+        <v>59070</v>
+      </c>
+      <c r="O3" s="4" t="n">
+        <f aca="false">M3/N3</f>
+        <v>0.00352124597934654</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="n">
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="n">
         <v>0.45</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4" t="n">
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5" t="n">
         <v>0.45</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I4" s="5" t="n">
         <v>0.55</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="6" t="n">
         <v>0.001342</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="5" t="n">
         <v>0.9</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="6" t="n">
         <v>0.000575</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <v>620</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <v>486440</v>
+      </c>
+      <c r="O4" s="4" t="n">
+        <f aca="false">M4/N4</f>
+        <v>0.00127456623632925</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="n">
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="n">
         <v>0.45</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4" t="n">
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="n">
         <v>0.45</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="5" t="n">
         <v>0.55</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="6" t="n">
         <v>0.001138</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="5" t="n">
         <v>0.9</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="6" t="n">
         <v>0.000831</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>635</v>
+      </c>
+      <c r="N5" s="7" t="n">
+        <v>486440</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <f aca="false">M5/N5</f>
+        <v>0.00130540251624044</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -549,128 +622,128 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="6" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="21.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="14" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="8" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="8" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="8" width="21.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="14" style="8" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="B1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="F2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="H2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="I2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="J2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="K2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="L2" s="9" t="s">
         <v>30</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="11" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="8" t="n">
+      <c r="E3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="L3" s="8" t="n">
+      <c r="L3" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="M3" s="8" t="n">
+      <c r="M3" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="8" t="n">
+      <c r="N3" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="O3" s="9" t="n">
+      <c r="O3" s="11" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Version Feb 15, 2022
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/based_modeling_trial.xlsx
+++ b/data_driven/modeling/output/based_modeling_trial.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t xml:space="preserve">Param ID</t>
   </si>
@@ -131,10 +131,10 @@
     <t xml:space="preserve">gini</t>
   </si>
   <si>
+    <t xml:space="preserve">sqrt</t>
+  </si>
+  <si>
     <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sqrt</t>
   </si>
 </sst>
 </file>
@@ -147,11 +147,12 @@
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -170,6 +171,12 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -236,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -253,6 +260,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +277,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,10 +377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q16" activeCellId="0" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,7 +424,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -445,147 +460,291 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="6" t="n">
         <v>0.4</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="6" t="n">
         <v>0.77</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="6" t="n">
         <v>0.4</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="6" t="n">
         <v>0.77</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="J3" s="6" t="n">
+      <c r="J3" s="7" t="n">
         <v>0.001493</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="6" t="n">
         <v>0.9</v>
       </c>
-      <c r="L3" s="6" t="n">
+      <c r="L3" s="7" t="n">
         <v>0.001789</v>
       </c>
-      <c r="M3" s="4" t="n">
-        <v>208</v>
-      </c>
-      <c r="N3" s="4" t="n">
+      <c r="M3" s="5" t="n">
+        <v>202</v>
+      </c>
+      <c r="N3" s="5" t="n">
         <v>59070</v>
       </c>
-      <c r="O3" s="4" t="n">
+      <c r="O3" s="5" t="n">
         <f aca="false">M3/N3</f>
-        <v>0.00352124597934654</v>
+        <v>0.00341967157609616</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="n">
+      <c r="A4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="6" t="n">
         <v>0.45</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>0.8</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="6" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>0.001342</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L4" s="7" t="n">
+        <v>0.000575</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>593</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>486440</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <f aca="false">M4/N4</f>
+        <v>0.0012190609324891</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="n">
         <v>0.45</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="E5" s="6" t="n">
         <v>0.8</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="6" t="n">
         <v>0.55</v>
       </c>
-      <c r="J4" s="6" t="n">
-        <v>0.001342</v>
-      </c>
-      <c r="K4" s="5" t="n">
+      <c r="J5" s="7" t="n">
+        <v>0.001138</v>
+      </c>
+      <c r="K5" s="6" t="n">
         <v>0.9</v>
       </c>
-      <c r="L4" s="6" t="n">
-        <v>0.000575</v>
-      </c>
-      <c r="M4" s="4" t="n">
-        <v>620</v>
-      </c>
-      <c r="N4" s="4" t="n">
+      <c r="L5" s="7" t="n">
+        <v>0.000831</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>608</v>
+      </c>
+      <c r="N5" s="8" t="n">
         <v>486440</v>
       </c>
-      <c r="O4" s="4" t="n">
-        <f aca="false">M4/N4</f>
-        <v>0.00127456623632925</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="O5" s="5" t="n">
+        <f aca="false">M5/N5</f>
+        <v>0.0012498972124003</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D6" s="5" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="I6" s="5" t="n">
         <v>0.45</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="J6" s="5" t="n">
+        <v>0.001265</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0.000204</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>3830</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>285888</v>
+      </c>
+      <c r="O6" s="5" t="n">
+        <f aca="false">M6/N6</f>
+        <v>0.0133968547123349</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="5" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="J5" s="6" t="n">
-        <v>0.001138</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="L5" s="6" t="n">
-        <v>0.000831</v>
-      </c>
-      <c r="M5" s="4" t="n">
-        <v>635</v>
-      </c>
-      <c r="N5" s="7" t="n">
-        <v>486440</v>
-      </c>
-      <c r="O5" s="4" t="n">
-        <f aca="false">M5/N5</f>
-        <v>0.00130540251624044</v>
+      <c r="G7" s="5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>0.001966</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>0.000211</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>1897</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>285578</v>
+      </c>
+      <c r="O7" s="5" t="n">
+        <f aca="false">M7/N7</f>
+        <v>0.00664266855289973</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>0.000865</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>0.000183</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>1888</v>
+      </c>
+      <c r="N8" s="5" t="n">
+        <v>286112</v>
+      </c>
+      <c r="O8" s="5" t="n">
+        <f aca="false">M8/N8</f>
+        <v>0.0065988144502852</v>
       </c>
     </row>
   </sheetData>
@@ -617,133 +776,133 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="8" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="8" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="8" width="21.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="14" style="8" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="10" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="10" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="10" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="10" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="10" width="21.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="14" style="10" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="n">
+      <c r="A3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="n">
+        <v>200</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="10" t="n">
+      <c r="I3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="10" t="n">
+      <c r="K3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="M3" s="10" t="n">
+      <c r="M3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="10" t="n">
+      <c r="N3" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="O3" s="11" t="n">
+      <c r="O3" s="13" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>